<commit_message>
Add init proces and excel procees
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bot\Documents\UiPath\REF_Proyect_CursoRPA\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52442\Documents\UiPath\REF-UIpath\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB7CFF1-43B9-4B49-891A-03C518B4E00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C46636-AC22-4A97-B2AC-84AC4D6454AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="1320" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -172,9 +172,6 @@
     <t>NombreArchivoInsumo</t>
   </si>
   <si>
-    <t>PalabrasClaves.txt</t>
-  </si>
-  <si>
     <t>Nombre del archivo TXT que contiene las palabras claves, nuestro archivo insumo</t>
   </si>
   <si>
@@ -221,6 +218,9 @@
   </si>
   <si>
     <t>Correo de las personas que deben recibir el reporte.</t>
+  </si>
+  <si>
+    <t>palabrasClaves.txt</t>
   </si>
 </sst>
 </file>
@@ -300,7 +300,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -598,11 +598,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -693,43 +693,43 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
         <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>465</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1735,7 +1735,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -1805,7 +1805,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -2894,11 +2894,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -2944,35 +2944,35 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>